<commit_message>
Add Test data and test functions
</commit_message>
<xml_diff>
--- a/testdata/SampleAssessmentResult-5.xlsx
+++ b/testdata/SampleAssessmentResult-5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Apple/Documents/Google-Sync/SWEN90014 Master Project/Project/swen90014-2019-rv-quoll/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5E884C-AED7-1549-97C0-F48C280E1F53}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3556BBB-264E-8A41-A713-51CFF962E0B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -2018,25 +2018,25 @@
         <v>689</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>